<commit_message>
- Added a new Register to easy access very important info inside a DataManager (it haves a Save All Data Funcionality still need a try) - Added a Basic Map system linked to the Register - Deleted LevelManager to a simplified GameState Manager where everything go together
 * Refactorize Object Prefab Instantiation from tiled Convention,
Using something more intuitive like type Configs inside Tiled 0.9 = DONE
 * Rebuild Tiled Example Level Objects: Mono, Dengue, Gaucho, etc = DONE

-> Next Goals:

 * Add Player level Spawn reading (a feature too)                 = WIP
 * Add Warp system level like: Input -> A ... Output -> A ( Door -> WarpTo: Id, Warp -> WarpTo: "File...tmx") = WIP
 * Edit Items and projectiles TileSets...
</commit_message>
<xml_diff>
--- a/TiledProperties.xlsx
+++ b/TiledProperties.xlsx
@@ -467,6 +467,55 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">auto-configurada por default según profundidad, van dos numeros enteros separados por coma  (o fraccionarios con punto) sino se considera como </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">un solo valor para el Eje </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          (y para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y = 0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">(0, 0) por default, van dos numeros separados por coma           (o fraccionarios con punto) sino se considera como  </t>
     </r>
     <r>
@@ -503,6 +552,9 @@
     <t xml:space="preserve"> RepeatX</t>
   </si>
   <si>
+    <t>NoRepeat</t>
+  </si>
+  <si>
     <r>
       <t>modo "</t>
     </r>
@@ -529,54 +581,14 @@
     </r>
   </si>
   <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>(PixelPerfect por default) propiedad exclusiva del modo    "Size = Original" cuando la textura es menor que el viewport esta se tilea en el eje indicado hasta cubrir todo el area libre y desactivando el tiling en el eje opuesto.   (usar valor Single para desactivarlo en ambos ejes)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">auto-configurada por default según profundidad, van dos numeros enteros separados por coma  (o fraccionarios con punto) sino se considera como un solo valor para el Eje </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">          (y para </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Y = 0)</t>
-    </r>
+    <t>(PixelPerfect por default) propiedad exclusiva del modo    "Size = Original" cuando la textura es menor que el viewport esta se tilea en el eje indicado hasta cubrir todo el area libre y desactivando el tiling en el eje opuesto.  (usar NoRepeat para desactivar ambos ejes a la vez)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,13 +621,6 @@
     <font>
       <b/>
       <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1104,7 +1109,7 @@
   <dimension ref="A2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1153,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
@@ -1235,7 +1240,7 @@
       <c r="D14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,7 +1281,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
@@ -1285,19 +1290,18 @@
     <row r="19" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
       <c r="C20" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" s="24"/>
-      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="20"/>
@@ -1314,8 +1318,8 @@
       <c r="C22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>47</v>
+      <c r="D22" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="6"/>
@@ -1329,7 +1333,7 @@
         <v>31</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>

</xml_diff>

<commit_message>
* Add moving platform feature...                           = DONE  * Add Player level Spawn reading (a feature too)           = DONE  * Add Warp system level like: Input -> A ... Output -> A   = DONE  * FlyPlatforms                                             = DONE  * Characters Dialog & Conversations Tiled Parsing          = DONE
-> Next Goals:
 * Test ConversationManager y Improve more features         = WIP
 * Edit Items and projectiles TileSets...
 * Enemy BIG BOSSES IA!:
			- Teju Yagua
			- Yasi Yatere
			- SNAKES
  			- AO AO
 * PLAYER SUPER POWERS: 
	- Caña X1, X2 Increment
	- Whistler
	- Smallability
 * Re-Arrange TileManager uber-grow in smaller sub-Managers: ObjectManager, ScrollManager, etc
</commit_message>
<xml_diff>
--- a/TiledProperties.xlsx
+++ b/TiledProperties.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
   <si>
     <t>PROPERTIES IN TILED:</t>
   </si>
@@ -582,6 +582,99 @@
   </si>
   <si>
     <t>(PixelPerfect por default) propiedad exclusiva del modo    "Size = Original" cuando la textura es menor que el viewport esta se tilea en el eje indicado hasta cubrir todo el area libre y desactivando el tiling en el eje opuesto.  (usar NoRepeat para desactivar ambos ejes a la vez)</t>
+  </si>
+  <si>
+    <t>Objects Types_</t>
+  </si>
+  <si>
+    <t>Dengue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> type</t>
+  </si>
+  <si>
+    <t>Gaucho</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> …</t>
+  </si>
+  <si>
+    <t>Mono</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bichejos de mala vida que aparte de molestar al Player no tienen importancia</t>
+  </si>
+  <si>
+    <t>Door / Warp</t>
+  </si>
+  <si>
+    <t>Nombre / Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Target</t>
+  </si>
+  <si>
+    <t>CheckPoint</t>
+  </si>
+  <si>
+    <t>Punto de llegada, si se especifica "Start" desde allí se empieza a jugar en la carga de cada nuevo nivel sino esquina izquierda</t>
+  </si>
+  <si>
+    <t>Id de destino a cualquier Warp dentro del  mismo mapa, se puede cargar otros mapas también poniendo por ejemplo: "/Levels/NivelX.tmx" y con "Exit" se vuelve al Mapa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Opcional / Start</t>
+  </si>
+  <si>
+    <t>Opcional / "file.tmx" / Exit</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Propiedades</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Valores Posibles:</t>
+  </si>
+  <si>
+    <t>Todos los Sitios de Warp y Doors registran automaticamente la ultima posición del Player en cada Mundo, Si no se especifica Ni Id ni Target esta será su unica función.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los Warps pueden crearse con Objetos de un Modulo o con Volumenes de Area Extendidas (Muy utiles para cubrír mejor)</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ( -2, 5, 0 )</t>
+  </si>
+  <si>
+    <t>velocidad (decimales siempre con punto)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lugar de destino de la plataforma que circula a partír de origen de posición en tiled </t>
+  </si>
+  <si>
+    <t>FlyPlatformA / FlyPlatformB / FlyPlatformC</t>
+  </si>
+  <si>
+    <t>Personaje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nameid </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> conversacion1</t>
+  </si>
+  <si>
+    <t>cada personaje tiene sus propias charlas y subcharlas</t>
   </si>
 </sst>
 </file>
@@ -628,7 +721,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -653,8 +746,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -727,11 +826,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -778,28 +952,91 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1106,10 +1343,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H33"/>
+  <dimension ref="A2:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,6 +1355,7 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1178,7 +1416,7 @@
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="37" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -1191,7 +1429,7 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
@@ -1200,7 +1438,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="12" t="s">
         <v>9</v>
       </c>
@@ -1244,7 +1482,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="15" t="s">
@@ -1255,7 +1493,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="12" t="s">
         <v>14</v>
       </c>
@@ -1265,7 +1503,7 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="37" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -1276,7 +1514,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="17" t="s">
         <v>21</v>
       </c>
@@ -1288,27 +1526,27 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
+      <c r="B19" s="38"/>
       <c r="C19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="42" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="24"/>
+      <c r="D20" s="43"/>
     </row>
     <row r="21" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="25"/>
+      <c r="D21" s="44"/>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1371,11 +1609,11 @@
       <c r="A26" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1385,16 +1623,176 @@
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="6"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="28"/>
+    </row>
+    <row r="31" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="34"/>
+    </row>
+    <row r="33" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="35"/>
+      <c r="E33" s="36"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
+    </row>
+    <row r="35" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="38"/>
+      <c r="C37" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="39"/>
+      <c r="C38" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="26"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="2:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="46"/>
+      <c r="C40" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B36:B38"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D31:E33"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="91" fitToWidth="0" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
* Add Player level Spawn reading (a feature too)           = DONE  * Add Warp system level like: Input -> A ... Output -> A   = DONE + Setup A Dictionary of Keys Strings + Vector3 Values for save up all the last level's checkpoints  * Characters Dialog & Conversations Tiled Parsing          = DONE  * Test ConversationManager y Improve more features         = DONE + Improved Comic Balloon Id Following and a less Gameplay invasive Dialog system (Now you can just keep running to avoid dialog, should not! but whatever..)
-> Next Goals:
 * Edit Items and projectiles TileSets...
 * Enemy BIG BOSSES IA!:
			- Teju Yagua
			- Yasi Yatere
			- SNAKES
  			- AO AO
 * PLAYER SUPER POWERS: 
	- Caña X1, X2 Increment
	- Whistler
	- Smallability
 * Re-Arrange TileManager uber-grow in smaller sub-Managers: ObjectManager, ScrollManager, etc
</commit_message>
<xml_diff>
--- a/TiledProperties.xlsx
+++ b/TiledProperties.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="89">
   <si>
     <t>PROPERTIES IN TILED:</t>
   </si>
@@ -665,16 +665,60 @@
     <t>FlyPlatformA / FlyPlatformB / FlyPlatformC</t>
   </si>
   <si>
-    <t>Personaje</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nameid </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> conversacion1</t>
-  </si>
-  <si>
     <t>cada personaje tiene sus propias charlas y subcharlas</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nombre bicho </t>
+  </si>
+  <si>
+    <t>nameid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clavel, fernando, kurupi</t>
+  </si>
+  <si>
+    <t>opción para cambiar archivo de dialogos por default</t>
+  </si>
+  <si>
+    <t>Conversation1.xml</t>
+  </si>
+  <si>
+    <t>"Comienzo", "Ganaste"</t>
+  </si>
+  <si>
+    <t>oneShot</t>
+  </si>
+  <si>
+    <t>por default true, si se especifica el Jugador entra en dialogo automaticamente al hacer contacto por primera vez sino es necesario hacer para arriba (como entrando en una puerta ) para iniciar una conversación luego.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mmh</t>
+  </si>
+  <si>
+    <t>Detalles</t>
+  </si>
+  <si>
+    <t>Personajes con Dialogo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tipo de subcharla asignado (se puede variar entre muchas para en un mismo archivo y mismo personaje) poner las mayusculas con </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exactitud</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -905,7 +949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -959,27 +1003,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1009,34 +1083,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1343,10 +1396,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H42"/>
+  <dimension ref="A2:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,7 +1408,7 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1416,7 +1469,7 @@
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -1429,7 +1482,7 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1491,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="12" t="s">
         <v>9</v>
       </c>
@@ -1449,6 +1502,7 @@
       <c r="G10" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1482,7 +1536,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="15" t="s">
@@ -1493,7 +1547,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="12" t="s">
         <v>14</v>
       </c>
@@ -1503,7 +1557,7 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="15" t="s">
@@ -1514,7 +1568,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="17" t="s">
         <v>21</v>
       </c>
@@ -1526,27 +1580,27 @@
       <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="43"/>
+      <c r="D20" s="33"/>
     </row>
     <row r="21" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="44"/>
+      <c r="D21" s="34"/>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1609,11 +1663,11 @@
       <c r="A26" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1633,169 +1687,221 @@
       <c r="C30" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="28"/>
-    </row>
-    <row r="31" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="38"/>
+    </row>
+    <row r="31" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="32"/>
-    </row>
-    <row r="32" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="42"/>
+    </row>
+    <row r="32" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13" t="s">
         <v>51</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34"/>
-    </row>
-    <row r="33" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="43"/>
+      <c r="E32" s="44"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="36"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="45"/>
+      <c r="E33" s="46"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-    </row>
-    <row r="35" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="39"/>
+      <c r="E34" s="40"/>
+    </row>
+    <row r="35" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="20" t="s">
-        <v>67</v>
+      <c r="D35" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>65</v>
       </c>
       <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="37" t="s">
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="21" t="s">
         <v>61</v>
       </c>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="2:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="38"/>
-      <c r="C37" s="23" t="s">
+    <row r="37" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="47"/>
+      <c r="C37" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="39"/>
-      <c r="C38" s="23" t="s">
+    <row r="38" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="31"/>
+      <c r="C38" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="26"/>
+      <c r="E38" s="36"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="2:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="45" t="s">
+    <row r="39" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="21" t="s">
         <v>71</v>
       </c>
+      <c r="G39" s="6"/>
       <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="46"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="28"/>
       <c r="C40" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
+    <row r="41" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="E41" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="27"/>
+      <c r="C42" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D42" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="14"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="22" t="s">
-        <v>61</v>
+      <c r="D43" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B44" s="28"/>
+      <c r="C44" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="14"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="14"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+    </row>
+    <row r="49" spans="4:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D49" s="24" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B21"/>
+  <mergeCells count="12">
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D31:E33"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B21"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="91" fitToWidth="0" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="27" max="16383" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
 

</xml_diff>